<commit_message>
UPDATE DATA AND SCRIPTS
updated data after correction, scripts and lw_pars to add other reliable species for l and g estimates from post_dist a b
</commit_message>
<xml_diff>
--- a/OnBoard/data/fogli_cala/StationTablet_22.xlsx
+++ b/OnBoard/data/fogli_cala/StationTablet_22.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\OneDrive - CNR\CNR\SoleMon\solemon2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f.luzi\OneDrive - CNR\CNR\SoleMon\solemon2024\access_da_modificare\SoleMon_project-main\OnBoard\data\fogli_cala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDB7B10B-466D-3344-B225-2D7AB97F9CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Station" sheetId="1" r:id="rId1"/>
     <sheet name="NotesCala" sheetId="2" r:id="rId2"/>
     <sheet name="Samples onboard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>WindDirection</t>
   </si>
@@ -202,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -635,37 +634,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7421875" style="13"/>
-    <col min="2" max="2" width="13.85546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.87109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.68359375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="9.28125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.0859375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.953125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="7.3984375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.2578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.8359375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="13"/>
+    <col min="2" max="2" width="13.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10" style="6" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="6" customWidth="1"/>
     <col min="14" max="14" width="12.77734375" style="6" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="6" customWidth="1"/>
-    <col min="17" max="17" width="13.44921875" style="6" customWidth="1"/>
-    <col min="18" max="18" width="8.47265625" style="6" customWidth="1"/>
-    <col min="19" max="21" width="8.609375" style="6"/>
-    <col min="22" max="22" width="13.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" style="6" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="8.44140625" style="6" customWidth="1"/>
+    <col min="19" max="21" width="8.5546875" style="6"/>
+    <col min="22" max="22" width="13.21875" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
@@ -733,7 +732,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>22</v>
       </c>
@@ -801,12 +800,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="22:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
@@ -814,7 +813,7 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" spans="22:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="22:27" x14ac:dyDescent="0.3">
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
@@ -828,26 +827,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7421875" style="9"/>
-    <col min="2" max="3" width="11.296875" style="6" customWidth="1"/>
-    <col min="4" max="5" width="11.703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.23828125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="13.85546875" style="6" customWidth="1"/>
-    <col min="9" max="10" width="10.4921875" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.8359375" style="17" customWidth="1"/>
-    <col min="12" max="12" width="11.02734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="9"/>
+    <col min="2" max="3" width="11.33203125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="6" customWidth="1"/>
+    <col min="7" max="8" width="13.88671875" style="6" customWidth="1"/>
+    <col min="9" max="10" width="10.44140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="17" customWidth="1"/>
+    <col min="12" max="12" width="11" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -885,7 +884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <f>Station!A2</f>
         <v>22</v>
@@ -915,481 +914,481 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>Station!A3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f>Station!A4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f>Station!A5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f>Station!A6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f>Station!A7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f>Station!A8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f>Station!A9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f>Station!A10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f>Station!A11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <f>Station!A12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <f>Station!A13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <f>Station!A14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <f>Station!A15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f>Station!A16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <f>Station!A17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <f>Station!A18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f>Station!A19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <f>Station!A20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <f>Station!A21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <f>Station!A22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <f>Station!A23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <f>Station!A24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <f>Station!A25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <f>Station!A26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <f>Station!A27</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <f>Station!A28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <f>Station!A29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <f>Station!A30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <f>Station!A31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <f>Station!A32</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <f>Station!A33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <f>Station!A34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <f>Station!A35</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <f>Station!A36</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <f>Station!A37</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <f>Station!A38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <f>Station!A39</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <f>Station!A40</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <f>Station!A41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <f>Station!A42</f>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <f>Station!A43</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <f>Station!A44</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <f>Station!A45</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <f>Station!A46</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <f>Station!A47</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <f>Station!A48</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <f>Station!A49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <f>Station!A50</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <f>Station!A51</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <f>Station!A52</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <f>Station!A53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <f>Station!A54</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="9">
         <f>Station!A55</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <f>Station!A56</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <f>Station!A57</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <f>Station!A58</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <f>Station!A59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <f>Station!A60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="9">
         <f>Station!A61</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="9">
         <f>Station!A62</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="9">
         <f>Station!A63</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="9">
         <f>Station!A64</f>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
         <f>Station!A65</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <f>Station!A66</f>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="9">
         <f>Station!A67</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="9">
         <f>Station!A68</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="9">
         <f>Station!A69</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="9">
         <f>Station!A70</f>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="9">
         <f>Station!A71</f>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="9">
         <f>Station!A72</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="9">
         <f>Station!A73</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="9">
         <f>Station!A74</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="9">
         <f>Station!A75</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="9">
         <f>Station!A76</f>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="9">
         <f>Station!A77</f>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="9">
         <f>Station!A78</f>
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <f>Station!A79</f>
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="9">
         <f>Station!A80</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="9">
         <f>Station!A81</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="9">
         <f>Station!A82</f>
         <v>0</v>
@@ -1401,21 +1400,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{639A9272-1023-F34A-8D2B-32933A221EB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="5" width="8.609375" style="18"/>
-    <col min="6" max="6" width="10.89453125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.5546875" style="18"/>
+    <col min="6" max="6" width="10.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1446,7 +1445,7 @@
         <v>46</v>
       </c>
       <c r="C2" s="18">
-        <v>38.299999999999997</v>
+        <v>383</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>45</v>
@@ -1455,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="18">
-        <v>41.2</v>
+        <v>412</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>45</v>
@@ -1472,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="18">
-        <v>37.700000000000003</v>
+        <v>377</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>45</v>
@@ -1489,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="18">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="F5" s="18">
         <v>2.4</v>

</xml_diff>